<commit_message>
Got the error working
</commit_message>
<xml_diff>
--- a/Exp 1 (voltage to speed) data files/ASEN 2002_1030_8_WTData.xlsx
+++ b/Exp 1 (voltage to speed) data files/ASEN 2002_1030_8_WTData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Documents/College Documents/Sophomore Year/Intro to Thermo:Aero/ASEN2002_Lab2/Exp 1 (voltage to speed) data files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD0C7BB8-743B-F543-8E2F-069ACFEA5C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{03F28B3C-B9A9-2349-B852-0F3EC4E989A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500"/>
+    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASEN 2002_1030_8_WTData" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -954,10 +954,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M101"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1091,7 +1093,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M2">
-        <v>-4.758</v>
+        <v>0.5</v>
       </c>
       <c r="N2">
         <v>3.573</v>
@@ -1180,7 +1182,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M3">
-        <v>-4.758</v>
+        <v>0.5</v>
       </c>
       <c r="N3">
         <v>4.6900000000000004</v>
@@ -1269,7 +1271,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M4">
-        <v>-4.5419999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="N4">
         <v>3.9089999999999998</v>
@@ -1358,7 +1360,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M5">
-        <v>-4.8659999999999997</v>
+        <v>0.5</v>
       </c>
       <c r="N5">
         <v>3.7970000000000002</v>
@@ -1447,7 +1449,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M6">
-        <v>-4.4340000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="N6">
         <v>3.2389999999999999</v>
@@ -1536,7 +1538,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M7">
-        <v>-4.3259999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="N7">
         <v>3.7970000000000002</v>
@@ -1625,7 +1627,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M8">
-        <v>-5.0830000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="N8">
         <v>4.3550000000000004</v>
@@ -1714,7 +1716,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M9">
-        <v>-4.3259999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="N9">
         <v>4.4669999999999996</v>
@@ -1803,7 +1805,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M10">
-        <v>-5.0830000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="N10">
         <v>3.5739999999999998</v>
@@ -1892,7 +1894,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M11">
-        <v>-4.8659999999999997</v>
+        <v>0.5</v>
       </c>
       <c r="N11">
         <v>4.1319999999999997</v>
@@ -1981,7 +1983,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M12">
-        <v>-4.4340000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="N12">
         <v>4.0199999999999996</v>
@@ -2070,7 +2072,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M13">
-        <v>-5.0830000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="N13">
         <v>4.3550000000000004</v>
@@ -2159,7 +2161,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M14">
-        <v>-5.0830000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="N14">
         <v>4.1319999999999997</v>
@@ -2248,7 +2250,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M15">
-        <v>-4.9740000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="N15">
         <v>4.1319999999999997</v>
@@ -2337,7 +2339,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M16">
-        <v>-4.5419999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="N16">
         <v>3.4620000000000002</v>
@@ -2426,7 +2428,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M17">
-        <v>-5.1909999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="N17">
         <v>4.1319999999999997</v>
@@ -2515,7 +2517,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M18">
-        <v>-4.5410000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="N18">
         <v>3.5739999999999998</v>
@@ -2604,7 +2606,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M19">
-        <v>-6.1630000000000003</v>
+        <v>0.5</v>
       </c>
       <c r="N19">
         <v>4.5789999999999997</v>
@@ -2693,7 +2695,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M20">
-        <v>-4.8659999999999997</v>
+        <v>0.5</v>
       </c>
       <c r="N20">
         <v>4.3550000000000004</v>
@@ -2782,7 +2784,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M21">
-        <v>-4.9740000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="N21">
         <v>2.7919999999999998</v>
@@ -2871,7 +2873,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M22">
-        <v>-5.407</v>
+        <v>2.5</v>
       </c>
       <c r="N22">
         <v>3.4620000000000002</v>
@@ -2960,7 +2962,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M23">
-        <v>-5.0830000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="N23">
         <v>4.1319999999999997</v>
@@ -3049,7 +3051,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M24">
-        <v>-4.758</v>
+        <v>2.5</v>
       </c>
       <c r="N24">
         <v>3.2389999999999999</v>
@@ -3138,7 +3140,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M25">
-        <v>-4.109</v>
+        <v>2.5</v>
       </c>
       <c r="N25">
         <v>3.4620000000000002</v>
@@ -3227,7 +3229,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M26">
-        <v>-4.9740000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="N26">
         <v>4.0199999999999996</v>
@@ -3316,7 +3318,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M27">
-        <v>-5.0830000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="N27">
         <v>4.2439999999999998</v>
@@ -3405,7 +3407,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M28">
-        <v>-4.2169999999999996</v>
+        <v>2.5</v>
       </c>
       <c r="N28">
         <v>4.3550000000000004</v>
@@ -3494,7 +3496,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M29">
-        <v>-4.4340000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="N29">
         <v>3.2389999999999999</v>
@@ -3583,7 +3585,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M30">
-        <v>-4.4340000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="N30">
         <v>3.9089999999999998</v>
@@ -3672,7 +3674,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M31">
-        <v>-4.3259999999999996</v>
+        <v>2.5</v>
       </c>
       <c r="N31">
         <v>4.5789999999999997</v>
@@ -3761,7 +3763,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M32">
-        <v>-5.6230000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="N32">
         <v>4.2439999999999998</v>
@@ -3850,7 +3852,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M33">
-        <v>-4.2169999999999996</v>
+        <v>2.5</v>
       </c>
       <c r="N33">
         <v>4.1319999999999997</v>
@@ -3939,7 +3941,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M34">
-        <v>-4.5419999999999998</v>
+        <v>2.5</v>
       </c>
       <c r="N34">
         <v>3.4620000000000002</v>
@@ -4028,7 +4030,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M35">
-        <v>-4.3259999999999996</v>
+        <v>2.5</v>
       </c>
       <c r="N35">
         <v>3.5739999999999998</v>
@@ -4117,7 +4119,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M36">
-        <v>-4.3259999999999996</v>
+        <v>2.5</v>
       </c>
       <c r="N36">
         <v>3.6850000000000001</v>
@@ -4206,7 +4208,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M37">
-        <v>-5.2990000000000004</v>
+        <v>2.5</v>
       </c>
       <c r="N37">
         <v>4.1319999999999997</v>
@@ -4295,7 +4297,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M38">
-        <v>-4.758</v>
+        <v>2.5</v>
       </c>
       <c r="N38">
         <v>4.2439999999999998</v>
@@ -4384,7 +4386,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M39">
-        <v>-4.758</v>
+        <v>2.5</v>
       </c>
       <c r="N39">
         <v>3.35</v>
@@ -4473,7 +4475,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M40">
-        <v>-4.5419999999999998</v>
+        <v>2.5</v>
       </c>
       <c r="N40">
         <v>3.4620000000000002</v>
@@ -4562,7 +4564,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M41">
-        <v>-4.2169999999999996</v>
+        <v>2.5</v>
       </c>
       <c r="N41">
         <v>4.1319999999999997</v>
@@ -4651,7 +4653,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M42">
-        <v>-5.407</v>
+        <v>4.5</v>
       </c>
       <c r="N42">
         <v>4.0199999999999996</v>
@@ -4740,7 +4742,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M43">
-        <v>-5.2990000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="N43">
         <v>4.5789999999999997</v>
@@ -4829,7 +4831,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M44">
-        <v>-4.3259999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="N44">
         <v>3.7970000000000002</v>
@@ -4918,7 +4920,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M45">
-        <v>-4.6500000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="N45">
         <v>4.0199999999999996</v>
@@ -5007,7 +5009,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M46">
-        <v>-4.3259999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="N46">
         <v>3.5739999999999998</v>
@@ -5096,7 +5098,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M47">
-        <v>-5.5149999999999997</v>
+        <v>4.5</v>
       </c>
       <c r="N47">
         <v>4.4669999999999996</v>
@@ -5185,7 +5187,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M48">
-        <v>-5.1909999999999998</v>
+        <v>4.5</v>
       </c>
       <c r="N48">
         <v>4.0199999999999996</v>
@@ -5274,7 +5276,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M49">
-        <v>-4.6500000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="N49">
         <v>3.9089999999999998</v>
@@ -5363,7 +5365,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M50">
-        <v>-4.4340000000000002</v>
+        <v>4.5</v>
       </c>
       <c r="N50">
         <v>3.35</v>
@@ -5452,7 +5454,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M51">
-        <v>-4.2169999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="N51">
         <v>4.2439999999999998</v>
@@ -5541,7 +5543,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M52">
-        <v>-4.758</v>
+        <v>4.5</v>
       </c>
       <c r="N52">
         <v>4.2439999999999998</v>
@@ -5630,7 +5632,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M53">
-        <v>-5.6230000000000002</v>
+        <v>4.5</v>
       </c>
       <c r="N53">
         <v>4.0199999999999996</v>
@@ -5719,7 +5721,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M54">
-        <v>-4.9740000000000002</v>
+        <v>4.5</v>
       </c>
       <c r="N54">
         <v>4.1319999999999997</v>
@@ -5808,7 +5810,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M55">
-        <v>-4.5419999999999998</v>
+        <v>4.5</v>
       </c>
       <c r="N55">
         <v>3.7970000000000002</v>
@@ -5897,7 +5899,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M56">
-        <v>-5.0830000000000002</v>
+        <v>4.5</v>
       </c>
       <c r="N56">
         <v>3.0150000000000001</v>
@@ -5986,7 +5988,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M57">
-        <v>-4.9740000000000002</v>
+        <v>4.5</v>
       </c>
       <c r="N57">
         <v>3.4620000000000002</v>
@@ -6075,7 +6077,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M58">
-        <v>-5.6230000000000002</v>
+        <v>4.5</v>
       </c>
       <c r="N58">
         <v>4.0199999999999996</v>
@@ -6164,7 +6166,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M59">
-        <v>-5.2990000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="N59">
         <v>4.4669999999999996</v>
@@ -6253,7 +6255,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M60">
-        <v>-4.6500000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="N60">
         <v>3.6850000000000001</v>
@@ -6342,7 +6344,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M61">
-        <v>-4.8659999999999997</v>
+        <v>4.5</v>
       </c>
       <c r="N61">
         <v>3.2389999999999999</v>
@@ -6431,7 +6433,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M62">
-        <v>-4.4340000000000002</v>
+        <v>6.5</v>
       </c>
       <c r="N62">
         <v>4.3550000000000004</v>
@@ -6520,7 +6522,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M63">
-        <v>-4.8659999999999997</v>
+        <v>6.5</v>
       </c>
       <c r="N63">
         <v>4.2439999999999998</v>
@@ -6609,7 +6611,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M64">
-        <v>-4.8659999999999997</v>
+        <v>6.5</v>
       </c>
       <c r="N64">
         <v>2.2330000000000001</v>
@@ -6698,7 +6700,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M65">
-        <v>-5.1909999999999998</v>
+        <v>6.5</v>
       </c>
       <c r="N65">
         <v>3.2389999999999999</v>
@@ -6787,7 +6789,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M66">
-        <v>-4.3259999999999996</v>
+        <v>6.5</v>
       </c>
       <c r="N66">
         <v>4.4669999999999996</v>
@@ -6876,7 +6878,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M67">
-        <v>-4.5419999999999998</v>
+        <v>6.5</v>
       </c>
       <c r="N67">
         <v>5.4720000000000004</v>
@@ -6965,7 +6967,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M68">
-        <v>-5.0830000000000002</v>
+        <v>6.5</v>
       </c>
       <c r="N68">
         <v>4.5789999999999997</v>
@@ -7054,7 +7056,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M69">
-        <v>-5.0830000000000002</v>
+        <v>6.5</v>
       </c>
       <c r="N69">
         <v>4.6900000000000004</v>
@@ -7143,7 +7145,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M70">
-        <v>-4.109</v>
+        <v>6.5</v>
       </c>
       <c r="N70">
         <v>3.2389999999999999</v>
@@ -7232,7 +7234,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M71">
-        <v>-5.407</v>
+        <v>6.5</v>
       </c>
       <c r="N71">
         <v>2.68</v>
@@ -7321,7 +7323,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M72">
-        <v>-4.758</v>
+        <v>6.5</v>
       </c>
       <c r="N72">
         <v>4.0199999999999996</v>
@@ -7410,7 +7412,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M73">
-        <v>-5.1909999999999998</v>
+        <v>6.5</v>
       </c>
       <c r="N73">
         <v>4.2439999999999998</v>
@@ -7499,7 +7501,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M74">
-        <v>-5.84</v>
+        <v>6.5</v>
       </c>
       <c r="N74">
         <v>3.7970000000000002</v>
@@ -7588,7 +7590,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M75">
-        <v>-4.2169999999999996</v>
+        <v>6.5</v>
       </c>
       <c r="N75">
         <v>5.36</v>
@@ -7677,7 +7679,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M76">
-        <v>-5.1909999999999998</v>
+        <v>6.5</v>
       </c>
       <c r="N76">
         <v>3.0150000000000001</v>
@@ -7766,7 +7768,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M77">
-        <v>-4.758</v>
+        <v>6.5</v>
       </c>
       <c r="N77">
         <v>3.1269999999999998</v>
@@ -7855,7 +7857,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M78">
-        <v>-5.1909999999999998</v>
+        <v>6.5</v>
       </c>
       <c r="N78">
         <v>3.4620000000000002</v>
@@ -7944,7 +7946,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M79">
-        <v>-3.7850000000000001</v>
+        <v>6.5</v>
       </c>
       <c r="N79">
         <v>3.5739999999999998</v>
@@ -8033,7 +8035,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M80">
-        <v>-3.8929999999999998</v>
+        <v>6.5</v>
       </c>
       <c r="N80">
         <v>4.8019999999999996</v>
@@ -8122,7 +8124,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M81">
-        <v>-4.8659999999999997</v>
+        <v>6.5</v>
       </c>
       <c r="N81">
         <v>4.2439999999999998</v>
@@ -8211,7 +8213,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M82">
-        <v>-4.5410000000000004</v>
+        <v>8.5</v>
       </c>
       <c r="N82">
         <v>4.5789999999999997</v>
@@ -8300,7 +8302,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M83">
-        <v>-4.649</v>
+        <v>8.5</v>
       </c>
       <c r="N83">
         <v>2.3450000000000002</v>
@@ -8389,7 +8391,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M84">
-        <v>-4.9740000000000002</v>
+        <v>8.5</v>
       </c>
       <c r="N84">
         <v>5.1369999999999996</v>
@@ -8478,7 +8480,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M85">
-        <v>-6.0549999999999997</v>
+        <v>8.5</v>
       </c>
       <c r="N85">
         <v>4.4669999999999996</v>
@@ -8567,7 +8569,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M86">
-        <v>-4.7569999999999997</v>
+        <v>8.5</v>
       </c>
       <c r="N86">
         <v>2.569</v>
@@ -8656,7 +8658,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M87">
-        <v>-4.0010000000000003</v>
+        <v>8.5</v>
       </c>
       <c r="N87">
         <v>4.6900000000000004</v>
@@ -8745,7 +8747,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M88">
-        <v>-5.5140000000000002</v>
+        <v>8.5</v>
       </c>
       <c r="N88">
         <v>4.3550000000000004</v>
@@ -8834,7 +8836,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M89">
-        <v>-6.2709999999999999</v>
+        <v>8.5</v>
       </c>
       <c r="N89">
         <v>2.68</v>
@@ -8923,7 +8925,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M90">
-        <v>-4.7569999999999997</v>
+        <v>8.5</v>
       </c>
       <c r="N90">
         <v>5.36</v>
@@ -9012,7 +9014,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M91">
-        <v>-6.92</v>
+        <v>8.5</v>
       </c>
       <c r="N91">
         <v>2.4569999999999999</v>
@@ -9101,7 +9103,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M92">
-        <v>-3.2440000000000002</v>
+        <v>8.5</v>
       </c>
       <c r="N92">
         <v>3.7970000000000002</v>
@@ -9190,7 +9192,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M93">
-        <v>-4.4329999999999998</v>
+        <v>8.5</v>
       </c>
       <c r="N93">
         <v>4.9139999999999997</v>
@@ -9279,7 +9281,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M94">
-        <v>-7.0279999999999996</v>
+        <v>8.5</v>
       </c>
       <c r="N94">
         <v>2.68</v>
@@ -9368,7 +9370,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M95">
-        <v>-5.5140000000000002</v>
+        <v>8.5</v>
       </c>
       <c r="N95">
         <v>4.0199999999999996</v>
@@ -9457,7 +9459,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M96">
-        <v>-3.8919999999999999</v>
+        <v>8.5</v>
       </c>
       <c r="N96">
         <v>3.2389999999999999</v>
@@ -9546,7 +9548,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M97">
-        <v>-4.5410000000000004</v>
+        <v>8.5</v>
       </c>
       <c r="N97">
         <v>4.6900000000000004</v>
@@ -9635,7 +9637,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M98">
-        <v>-5.5140000000000002</v>
+        <v>8.5</v>
       </c>
       <c r="N98">
         <v>3.35</v>
@@ -9724,7 +9726,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M99">
-        <v>-4.4329999999999998</v>
+        <v>8.5</v>
       </c>
       <c r="N99">
         <v>3.5739999999999998</v>
@@ -9813,7 +9815,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M100">
-        <v>-7.2439999999999998</v>
+        <v>8.5</v>
       </c>
       <c r="N100">
         <v>3.238</v>
@@ -9902,7 +9904,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="M101">
-        <v>-6.5949999999999998</v>
+        <v>8.5</v>
       </c>
       <c r="N101">
         <v>2.1219999999999999</v>

</xml_diff>